<commit_message>
Update with author-specific affiliations
</commit_message>
<xml_diff>
--- a/highly_cited_UNC_testinput.xlsx
+++ b/highly_cited_UNC_testinput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremy/Desktop/COVID_WFH_DATA/Neuroscience/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsimon/Desktop/Grants/CoPublication_Networks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C8CCCC7-AE9A-0041-92CD-116B23EE4E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CB4BA4-9811-2A41-8355-C20476538672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{E9B39631-A522-1B4B-AB3D-1ADBD234070A}"/>
+    <workbookView xWindow="380" yWindow="740" windowWidth="28040" windowHeight="16280" xr2:uid="{E9B39631-A522-1B4B-AB3D-1ADBD234070A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
-    <t>Faculty</t>
-  </si>
-  <si>
     <t>Hoadley K</t>
   </si>
   <si>
@@ -171,6 +168,9 @@
   </si>
   <si>
     <t>You W</t>
+  </si>
+  <si>
+    <t>University of North Carolina</t>
   </si>
 </sst>
 </file>
@@ -226,9 +226,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -266,7 +266,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -372,7 +372,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -514,7 +514,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -525,7 +525,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -535,244 +535,244 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
       <c r="C6" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
       <c r="C8" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
       <c r="C9" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
       <c r="C10" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
       <c r="C11" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
       <c r="C12" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
       <c r="C13" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
         <v>29</v>
       </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
       <c r="C15" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
-        <v>32</v>
-      </c>
       <c r="C16" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
         <v>33</v>
       </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
       <c r="C17" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
       <c r="C18" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
       <c r="C19" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
         <v>39</v>
       </c>
-      <c r="B20" t="s">
-        <v>40</v>
-      </c>
       <c r="C20" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
         <v>41</v>
       </c>
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
       <c r="C21" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
-        <v>44</v>
-      </c>
       <c r="C22" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>